<commit_message>
Update Languages excel file to include "Date".
</commit_message>
<xml_diff>
--- a/Documentation/Languages/Languages.xlsx
+++ b/Documentation/Languages/Languages.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="208">
   <si>
     <t>TESTO IN GUI</t>
   </si>
@@ -624,6 +624,30 @@
   </si>
   <si>
     <t>MENU PRINCIPAL</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>tableColDate.text</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>дата</t>
+  </si>
+  <si>
+    <t>تاريخ</t>
+  </si>
+  <si>
+    <t>日付</t>
   </si>
 </sst>
 </file>
@@ -728,7 +752,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -825,11 +849,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -890,9 +945,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -927,6 +979,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1209,10 +1275,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1241,16 +1307,16 @@
       <c r="F1" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="32" t="s">
         <v>131</v>
       </c>
       <c r="H1" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="I1" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="J1" s="39" t="s">
         <v>179</v>
       </c>
     </row>
@@ -1319,16 +1385,16 @@
       <c r="F4" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="33" t="s">
         <v>150</v>
       </c>
       <c r="I4" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="J4" s="39" t="s">
+      <c r="J4" s="38" t="s">
         <v>181</v>
       </c>
     </row>
@@ -1383,7 +1449,7 @@
       <c r="F6" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="G6" s="31" t="s">
+      <c r="G6" s="30" t="s">
         <v>146</v>
       </c>
       <c r="H6" s="24" t="s">
@@ -1466,10 +1532,10 @@
       <c r="F9" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="H9" s="34" t="s">
+      <c r="H9" s="33" t="s">
         <v>153</v>
       </c>
       <c r="I9" s="22" t="s">
@@ -1498,10 +1564,10 @@
       <c r="F10" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="G10" s="30" t="s">
+      <c r="G10" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="H10" s="34" t="s">
+      <c r="H10" s="33" t="s">
         <v>154</v>
       </c>
       <c r="I10" s="22" t="s">
@@ -1565,7 +1631,7 @@
       <c r="G12" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="H12" s="34" t="s">
+      <c r="H12" s="33" t="s">
         <v>156</v>
       </c>
       <c r="I12" s="22" t="s">
@@ -1594,13 +1660,13 @@
       <c r="F13" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="G13" s="32" t="s">
+      <c r="G13" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="H13" s="34" t="s">
+      <c r="H13" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="I13" s="37" t="s">
+      <c r="I13" s="36" t="s">
         <v>198</v>
       </c>
       <c r="J13" s="22" t="s">
@@ -1629,10 +1695,10 @@
       <c r="G14" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="H14" s="35" t="s">
+      <c r="H14" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="I14" s="37" t="s">
+      <c r="I14" s="36" t="s">
         <v>197</v>
       </c>
       <c r="J14" s="24" t="s">
@@ -1675,7 +1741,7 @@
       <c r="G16" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="H16" s="36" t="s">
+      <c r="H16" s="35" t="s">
         <v>159</v>
       </c>
       <c r="I16" s="21" t="s">
@@ -1780,10 +1846,10 @@
       <c r="G19" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="I19" s="37" t="s">
+      <c r="I19" s="36" t="s">
         <v>199</v>
       </c>
       <c r="J19" s="11" t="s">
@@ -1791,7 +1857,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -1828,7 +1894,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="19" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="19"/>
@@ -1842,19 +1908,19 @@
       <c r="J21" s="20"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="14" t="s">
         <v>105</v>
       </c>
       <c r="F22" s="14" t="str">
@@ -1865,7 +1931,7 @@
         <f>UPPER(G5)</f>
         <v>СТАТИ́СТИКА</v>
       </c>
-      <c r="H22" s="14" t="str">
+      <c r="H22" s="42" t="str">
         <f>UPPER(H5)</f>
         <v>إحصائية</v>
       </c>
@@ -1879,7 +1945,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="41" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -1902,7 +1968,7 @@
       <c r="G23" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="H23" s="11" t="str">
+      <c r="H23" s="43" t="str">
         <f>UPPER(H14)</f>
         <v>عَادَ</v>
       </c>
@@ -1916,7 +1982,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="41" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -1934,21 +2000,21 @@
       <c r="F24" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="G24" s="29" t="s">
+      <c r="G24" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="H24" s="34" t="s">
+      <c r="H24" s="44" t="s">
         <v>161</v>
       </c>
       <c r="I24" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="J24" s="39" t="s">
+      <c r="J24" s="38" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="41" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -1966,10 +2032,10 @@
       <c r="F25" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="G25" s="29" t="s">
+      <c r="G25" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="H25" s="34" t="s">
+      <c r="H25" s="44" t="s">
         <v>162</v>
       </c>
       <c r="I25" s="11" t="s">
@@ -1980,7 +2046,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="41" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -1995,97 +2061,129 @@
       <c r="E26" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="F26" s="24" t="s">
+      <c r="F26" s="22" t="s">
         <v>122</v>
       </c>
       <c r="G26" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="H26" s="35" t="s">
+      <c r="H26" s="44" t="s">
         <v>163</v>
       </c>
-      <c r="I26" s="13" t="s">
+      <c r="I26" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="J26" s="24" t="s">
+      <c r="J26" s="22" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="40" t="s">
+        <v>202</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="F27" s="45" t="s">
+        <v>201</v>
+      </c>
+      <c r="G27" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="H27" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="J27" s="24" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B29" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C29" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D29" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E29" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="F28" s="21" t="s">
+      <c r="F29" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="G28" s="27" t="s">
+      <c r="G29" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="H28" s="27" t="s">
+      <c r="H29" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="I28" s="10" t="s">
+      <c r="I29" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="J28" s="10" t="s">
+      <c r="J29" s="10" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B30" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C30" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D30" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E30" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F29" s="24" t="s">
+      <c r="F30" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="G29" s="24" t="s">
+      <c r="G30" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="H29" s="24" t="s">
+      <c r="H30" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="I29" s="13" t="s">
+      <c r="I30" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="J29" s="24" t="s">
+      <c r="J30" s="24" t="s">
         <v>196</v>
       </c>
     </row>

</xml_diff>